<commit_message>
SE BASIC ALL DONE
</commit_message>
<xml_diff>
--- a/circuits/mixed_feeder.xlsx
+++ b/circuits/mixed_feeder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshil\Desktop\4thyear\python\final code\circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947998AA-E259-43B6-9E67-D1A15D773720}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D453795E-7598-4F47-A27F-A22B8BA830A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="793" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="793" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dtypes" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="316">
   <si>
     <t>element</t>
   </si>
@@ -904,9 +904,6 @@
     <t>Bus RC6</t>
   </si>
   <si>
-    <t>Bus RC7</t>
-  </si>
-  <si>
     <t>Bus RC8</t>
   </si>
   <si>
@@ -955,9 +952,6 @@
     <t>Line RC5-RC6</t>
   </si>
   <si>
-    <t>Line RC6-RC7</t>
-  </si>
-  <si>
     <t>Line RC2-RC8</t>
   </si>
   <si>
@@ -1016,6 +1010,9 @@
   </si>
   <si>
     <t>CHP diesel 4rc</t>
+  </si>
+  <si>
+    <t>CHP diesel 5rc</t>
   </si>
 </sst>
 </file>
@@ -10014,7 +10011,7 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="A20:F21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10377,24 +10374,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
-        <v>290</v>
-      </c>
-      <c r="C19">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>195</v>
-      </c>
-      <c r="E19" t="s">
-        <v>196</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -10771,8 +10751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10829,7 +10809,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C2" t="s">
         <v>197</v>
@@ -10876,7 +10856,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C3" t="s">
         <v>197</v>
@@ -10903,7 +10883,7 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -10923,7 +10903,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C4" t="s">
         <v>197</v>
@@ -10950,7 +10930,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -10970,7 +10950,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" t="s">
         <v>197</v>
@@ -10997,7 +10977,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -11017,7 +10997,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" t="s">
         <v>197</v>
@@ -11044,7 +11024,7 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -11064,13 +11044,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C7" t="s">
         <v>197</v>
       </c>
       <c r="D7">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>54</v>
@@ -11111,13 +11091,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C8" t="s">
         <v>197</v>
       </c>
       <c r="D8">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E8">
         <v>55</v>
@@ -11138,7 +11118,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -11158,7 +11138,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C9" t="s">
         <v>197</v>
@@ -11185,7 +11165,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -11205,7 +11185,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C10" t="s">
         <v>197</v>
@@ -11217,7 +11197,7 @@
         <v>57</v>
       </c>
       <c r="F10">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G10">
         <v>0.16200000000000001</v>
@@ -11232,7 +11212,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -11252,7 +11232,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C11" t="s">
         <v>197</v>
@@ -11264,7 +11244,7 @@
         <v>58</v>
       </c>
       <c r="F11">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G11">
         <v>0.16200000000000001</v>
@@ -11279,7 +11259,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -11299,7 +11279,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C12" t="s">
         <v>197</v>
@@ -11346,7 +11326,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C13" t="s">
         <v>197</v>
@@ -11393,7 +11373,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C14" t="s">
         <v>197</v>
@@ -11405,7 +11385,7 @@
         <v>61</v>
       </c>
       <c r="F14">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G14">
         <v>0.16200000000000001</v>
@@ -11420,7 +11400,7 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -11440,13 +11420,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C15" t="s">
         <v>197</v>
       </c>
       <c r="D15">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E15">
         <v>62</v>
@@ -11467,7 +11447,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -11487,13 +11467,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C16" t="s">
         <v>197</v>
       </c>
       <c r="D16">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E16">
         <v>63</v>
@@ -11534,7 +11514,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C17" t="s">
         <v>197</v>
@@ -11577,51 +11557,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>307</v>
-      </c>
-      <c r="C18" t="s">
-        <v>197</v>
-      </c>
-      <c r="D18">
-        <v>64</v>
-      </c>
-      <c r="E18">
-        <v>65</v>
-      </c>
-      <c r="F18">
-        <v>0.03</v>
-      </c>
-      <c r="G18">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="H18">
-        <v>8.3199999999999996E-2</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>203</v>
-      </c>
-      <c r="O18" t="b">
-        <v>1</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -11750,7 +11686,7 @@
   <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11886,10 +11822,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C5" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -11916,10 +11852,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C6" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -11946,10 +11882,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C7" s="1">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -11976,10 +11912,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C8" s="1">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -12006,10 +11942,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C9" s="1">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -12036,10 +11972,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C10" s="1">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -12066,10 +12002,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C11" s="1">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -12096,10 +12032,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C12" s="1">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -12126,10 +12062,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C13" s="1">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -12152,78 +12088,26 @@
       <c r="U13" s="3"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>288</v>
-      </c>
-      <c r="C14" s="1">
-        <v>63</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="U14" s="3"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>289</v>
-      </c>
-      <c r="C15" s="1">
-        <v>64</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="U15" s="3"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="4"/>
       <c r="U16" s="3"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="C17" s="1"/>
       <c r="U17" s="3"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="C18" s="4"/>
       <c r="U18" s="3"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -12407,8 +12291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12451,10 +12335,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -12472,7 +12356,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -12483,10 +12367,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -12504,7 +12388,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -12515,10 +12399,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -12536,7 +12420,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -12547,10 +12431,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C5">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -12568,7 +12452,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -12579,10 +12463,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C6">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -12600,14 +12484,43 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.31</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>311</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -12691,10 +12604,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -12715,7 +12628,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M2">
         <v>7.0000000000000007E-2</v>

</xml_diff>

<commit_message>
ready to do flex
</commit_message>
<xml_diff>
--- a/circuits/mixed_feeder.xlsx
+++ b/circuits/mixed_feeder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshil\Desktop\4thyear\python\final code\circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D453795E-7598-4F47-A27F-A22B8BA830A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F27F0AC-0387-4C6B-B70A-F3C2D96131DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="793" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="793" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dtypes" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="314">
   <si>
     <t>element</t>
   </si>
@@ -1001,12 +1001,6 @@
   </si>
   <si>
     <t>CHP diesel</t>
-  </si>
-  <si>
-    <t>EV 4</t>
-  </si>
-  <si>
-    <t>EV</t>
   </si>
   <si>
     <t>CHP diesel 4rc</t>
@@ -10751,7 +10745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -12463,7 +12457,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C6">
         <v>64</v>
@@ -12495,7 +12489,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C7">
         <v>53</v>
@@ -12555,8 +12549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12600,39 +12594,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C2">
-        <v>62</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.04</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>313</v>
-      </c>
-      <c r="M2">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>